<commit_message>
CIERRE 22 AGO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="781">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2861,10 +2861,28 @@
     <t>POLLO-QUESOS-JAMON-SALCHICHA</t>
   </si>
   <si>
-    <t>HIERVAS-JAMON-QUESOS-POLLO-PALITOS</t>
-  </si>
-  <si>
     <t>PAN BCO-QUESOS-POLLO-CHORIZO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  </t>
+  </si>
+  <si>
+    <t>HIERBAS-JAMON-QUESOS-POLLO-PALITOS D QUESO</t>
+  </si>
+  <si>
+    <t>PASTOR--MAIZ-POLLO-QUESOS-ARABE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POLLO-QUESOS-</t>
+  </si>
+  <si>
+    <t>NOMINA # 27 Y Vac Dario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMINA # 27 </t>
+  </si>
+  <si>
+    <t>PASTOR-TOSTADAS-CHORIZO-CHISTORRA</t>
   </si>
 </sst>
 </file>
@@ -19503,8 +19521,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19829,7 +19847,7 @@
         <v>45112</v>
       </c>
       <c r="C9" s="33">
-        <v>18542.5</v>
+        <v>14760</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>773</v>
@@ -19838,34 +19856,34 @@
         <v>45112</v>
       </c>
       <c r="F9" s="36">
-        <v>133632</v>
+        <v>155261</v>
       </c>
       <c r="G9" s="37"/>
       <c r="H9" s="38">
         <v>45112</v>
       </c>
       <c r="I9" s="39">
-        <v>1533</v>
+        <v>1711</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="348"/>
       <c r="L9" s="49"/>
       <c r="M9" s="42">
-        <v>61007.5</v>
+        <f>81885+6611</f>
+        <v>88496</v>
       </c>
       <c r="N9" s="43">
-        <v>52549</v>
+        <v>51697</v>
       </c>
       <c r="P9" s="49">
         <f t="shared" si="0"/>
-        <v>133632</v>
+        <v>156664</v>
       </c>
       <c r="Q9" s="45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="46">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R9" s="282" t="s">
+        <v>774</v>
       </c>
       <c r="S9" s="459"/>
       <c r="T9" s="233"/>
@@ -19880,40 +19898,40 @@
         <v>45113</v>
       </c>
       <c r="C10" s="33">
-        <v>14760</v>
+        <v>18542.5</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E10" s="35">
         <v>45113</v>
       </c>
       <c r="F10" s="36">
-        <v>155261</v>
+        <v>133632</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="38">
         <v>45113</v>
       </c>
       <c r="I10" s="39">
-        <v>1711</v>
+        <v>1533</v>
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="54"/>
       <c r="L10" s="55"/>
       <c r="M10" s="42">
-        <v>81885</v>
+        <v>61007.5</v>
       </c>
       <c r="N10" s="43">
-        <v>51697</v>
+        <v>52549</v>
       </c>
       <c r="P10" s="49">
         <f t="shared" si="0"/>
-        <v>150053</v>
+        <v>133632</v>
       </c>
       <c r="Q10" s="45">
         <f t="shared" si="1"/>
-        <v>-5208</v>
+        <v>0</v>
       </c>
       <c r="R10" s="46">
         <v>0</v>
@@ -19930,29 +19948,37 @@
       <c r="B11" s="32">
         <v>45114</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="47"/>
+      <c r="C11" s="33">
+        <v>7981</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>776</v>
+      </c>
       <c r="E11" s="35">
         <v>45114</v>
       </c>
-      <c r="F11" s="36"/>
+      <c r="F11" s="36">
+        <v>147770</v>
+      </c>
       <c r="G11" s="37"/>
       <c r="H11" s="38">
         <v>45114</v>
       </c>
-      <c r="I11" s="39"/>
+      <c r="I11" s="39">
+        <v>3808</v>
+      </c>
       <c r="J11" s="52"/>
       <c r="K11" s="58"/>
       <c r="L11" s="49"/>
       <c r="M11" s="42">
-        <v>0</v>
+        <v>66409</v>
       </c>
       <c r="N11" s="43">
-        <v>0</v>
+        <v>69572</v>
       </c>
       <c r="P11" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147770</v>
       </c>
       <c r="Q11" s="45">
         <f t="shared" si="1"/>
@@ -19966,37 +19992,52 @@
       <c r="U11" s="233"/>
       <c r="V11" s="233"/>
     </row>
-    <row r="12" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="26.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="504" t="s">
         <v>656</v>
       </c>
       <c r="B12" s="32">
         <v>45115</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="47"/>
+      <c r="C12" s="33">
+        <v>6557</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>777</v>
+      </c>
       <c r="E12" s="35">
         <v>45115</v>
       </c>
-      <c r="F12" s="36"/>
+      <c r="F12" s="36">
+        <v>162679</v>
+      </c>
       <c r="G12" s="37"/>
       <c r="H12" s="38">
         <v>45115</v>
       </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="342"/>
-      <c r="L12" s="49"/>
+      <c r="I12" s="39">
+        <v>3945</v>
+      </c>
+      <c r="J12" s="40">
+        <v>45115</v>
+      </c>
+      <c r="K12" s="342" t="s">
+        <v>778</v>
+      </c>
+      <c r="L12" s="49">
+        <v>27219</v>
+      </c>
       <c r="M12" s="42">
-        <v>0</v>
+        <f>48444+2958</f>
+        <v>51402</v>
       </c>
       <c r="N12" s="43">
-        <v>0</v>
+        <v>73556</v>
       </c>
       <c r="O12" s="192"/>
       <c r="P12" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>162679</v>
       </c>
       <c r="Q12" s="45">
         <f t="shared" si="1"/>
@@ -20017,34 +20058,41 @@
       <c r="B13" s="32">
         <v>45116</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="33">
+        <v>21802</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>780</v>
+      </c>
       <c r="E13" s="35">
         <v>45116</v>
       </c>
-      <c r="F13" s="36"/>
+      <c r="F13" s="36">
+        <v>140546</v>
+      </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38">
         <v>45116</v>
       </c>
-      <c r="I13" s="39"/>
+      <c r="I13" s="39">
+        <v>1712</v>
+      </c>
       <c r="J13" s="40"/>
       <c r="K13" s="343"/>
       <c r="L13" s="49"/>
       <c r="M13" s="42">
-        <v>0</v>
+        <v>72370</v>
       </c>
       <c r="N13" s="43">
-        <v>0</v>
+        <v>44662</v>
       </c>
       <c r="O13" s="192"/>
       <c r="P13" s="49">
         <f>N13+M13+L13+I13+C13</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="45">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>140546</v>
+      </c>
+      <c r="Q13" s="45" t="s">
+        <v>10</v>
       </c>
       <c r="R13" s="46">
         <v>0</v>
@@ -20928,9 +20976,15 @@
       <c r="G35" s="37"/>
       <c r="H35" s="38"/>
       <c r="I35" s="39"/>
-      <c r="J35" s="374"/>
-      <c r="K35" s="373"/>
-      <c r="L35" s="375"/>
+      <c r="J35" s="374">
+        <v>45115</v>
+      </c>
+      <c r="K35" s="373" t="s">
+        <v>779</v>
+      </c>
+      <c r="L35" s="375">
+        <v>27714.5</v>
+      </c>
       <c r="M35" s="42">
         <v>0</v>
       </c>
@@ -21347,19 +21401,19 @@
       <c r="L49" s="49"/>
       <c r="M49" s="558">
         <f>SUM(M5:M40)</f>
-        <v>399600</v>
+        <v>596392</v>
       </c>
       <c r="N49" s="558">
         <f>SUM(N5:N40)</f>
-        <v>340834</v>
+        <v>528624</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>926095</v>
+        <v>1383701</v>
       </c>
       <c r="Q49" s="570">
         <f>SUM(Q5:Q40)</f>
-        <v>23764</v>
+        <v>28972</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -21438,7 +21492,7 @@
       <c r="L53" s="49"/>
       <c r="M53" s="536">
         <f>M49+N49</f>
-        <v>740434</v>
+        <v>1125016</v>
       </c>
       <c r="N53" s="537"/>
       <c r="P53" s="44"/>
@@ -21679,7 +21733,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>124967.5</v>
+        <v>161307.5</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -21687,7 +21741,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>899237</v>
+        <v>1350232</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -21695,7 +21749,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>9943.5</v>
+        <v>19408.5</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -21703,7 +21757,7 @@
       </c>
       <c r="L67" s="527">
         <f>SUM(L5:L65)-L26</f>
-        <v>50750</v>
+        <v>105683.5</v>
       </c>
       <c r="M67" s="150"/>
       <c r="N67" s="150"/>
@@ -21728,7 +21782,7 @@
       <c r="J69" s="154"/>
       <c r="K69" s="568">
         <f>I67+L67</f>
-        <v>60693.5</v>
+        <v>125092</v>
       </c>
       <c r="L69" s="569"/>
       <c r="M69" s="155"/>
@@ -21743,7 +21797,7 @@
       <c r="E70" s="560"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>713576</v>
+        <v>1063832.5</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
@@ -21762,7 +21816,7 @@
       <c r="J71" s="563"/>
       <c r="K71" s="564">
         <f>F73+F74+F75</f>
-        <v>3534127.31</v>
+        <v>3884383.81</v>
       </c>
       <c r="L71" s="564"/>
       <c r="M71" s="159"/>
@@ -21798,7 +21852,7 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>713576</v>
+        <v>1063832.5</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
@@ -21839,7 +21893,7 @@
       <c r="J75" s="556"/>
       <c r="K75" s="557">
         <f>K71+K73</f>
-        <v>402740.27</v>
+        <v>752996.77</v>
       </c>
       <c r="L75" s="557"/>
     </row>
@@ -21986,7 +22040,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q49:Q50"/>
     <mergeCell ref="M53:N53"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="B1:B2"/>
@@ -22008,6 +22061,7 @@
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
+    <mergeCell ref="Q49:Q50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 24 ago 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="783">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2886,6 +2886,9 @@
   </si>
   <si>
     <t>LONGANIZA-QUESOS-CHISTORRA-POLLO</t>
+  </si>
+  <si>
+    <t>BIMBO-QUESOS-MILANESA-PASTOR-RETAZO</t>
   </si>
 </sst>
 </file>
@@ -5576,6 +5579,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5651,39 +5690,6 @@
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5749,9 +5755,6 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9138,23 +9141,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -9164,24 +9167,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="536" t="s">
+      <c r="R3" s="548" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9196,14 +9199,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -9213,11 +9216,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="537"/>
+      <c r="R4" s="549"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -11052,11 +11055,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -11064,7 +11067,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -11085,10 +11088,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -11143,11 +11146,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -11572,26 +11575,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="555" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="556"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="557">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="558"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="549" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="549"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -11600,22 +11603,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="550" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="550"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="551" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="552"/>
-      <c r="K79" s="553">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="553"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -11656,11 +11659,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="554">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="553"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -11677,22 +11680,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="542" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="543"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="544" t="s">
+      <c r="I83" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="545"/>
-      <c r="K83" s="546">
+      <c r="J83" s="557"/>
+      <c r="K83" s="558">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="546"/>
+      <c r="L83" s="558"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -11839,12 +11842,6 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -11861,6 +11858,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13030,10 +13033,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="575" t="s">
+      <c r="I37" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="576"/>
+      <c r="J37" s="577"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -13052,8 +13055,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="577"/>
-      <c r="J38" s="578"/>
+      <c r="I38" s="578"/>
+      <c r="J38" s="579"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -13072,8 +13075,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="579"/>
-      <c r="J39" s="580"/>
+      <c r="I39" s="580"/>
+      <c r="J39" s="581"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -13631,10 +13634,10 @@
         <f>SUM(G3:G66)</f>
         <v>1542483.7999999996</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>113965</v>
@@ -13656,11 +13659,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -13671,7 +13674,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -14259,23 +14262,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -14285,27 +14288,27 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
         <v>509</v>
       </c>
-      <c r="R3" s="592" t="s">
+      <c r="R3" s="593" t="s">
         <v>3</v>
       </c>
     </row>
@@ -14320,14 +14323,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -14337,11 +14340,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="593"/>
+      <c r="R4" s="594"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -16397,11 +16400,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -16409,7 +16412,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -16442,10 +16445,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -16530,11 +16533,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -16863,26 +16866,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="555" t="s">
+      <c r="H69" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="556"/>
+      <c r="I69" s="568"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="557">
+      <c r="K69" s="569">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="558"/>
+      <c r="L69" s="570"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="549" t="s">
+      <c r="D70" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="549"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -16891,23 +16894,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="550" t="s">
+      <c r="D71" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="550"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="551" t="s">
+      <c r="I71" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="552"/>
-      <c r="K71" s="553">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="553"/>
+      <c r="L71" s="565"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -16949,11 +16952,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="554">
+      <c r="K73" s="566">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="553"/>
+      <c r="L73" s="565"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -16970,22 +16973,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="542" t="s">
+      <c r="D75" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="543"/>
+      <c r="E75" s="555"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="544" t="s">
+      <c r="I75" s="556" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="545"/>
-      <c r="K75" s="546">
+      <c r="J75" s="557"/>
+      <c r="K75" s="558">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="546"/>
+      <c r="L75" s="558"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -17133,6 +17136,12 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -17149,12 +17158,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -18324,10 +18327,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="575" t="s">
+      <c r="I37" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="576"/>
+      <c r="J37" s="577"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -18346,8 +18349,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="577"/>
-      <c r="J38" s="578"/>
+      <c r="I38" s="578"/>
+      <c r="J38" s="579"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -18366,8 +18369,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="579"/>
-      <c r="J39" s="580"/>
+      <c r="I39" s="580"/>
+      <c r="J39" s="581"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -18925,10 +18928,10 @@
         <f>SUM(G3:G66)</f>
         <v>1585182.9300000004</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>121417.2</v>
@@ -18950,11 +18953,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -18965,7 +18968,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -19527,8 +19530,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19554,23 +19557,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -19580,25 +19583,25 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
-      <c r="R3" s="592" t="s">
+      <c r="R3" s="593" t="s">
         <v>3</v>
       </c>
     </row>
@@ -19613,14 +19616,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -19630,11 +19633,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="593"/>
+      <c r="R4" s="594"/>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -20167,29 +20170,44 @@
       <c r="B15" s="32">
         <v>45118</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="33">
+        <v>13656</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>782</v>
+      </c>
       <c r="E15" s="35">
         <v>45118</v>
       </c>
-      <c r="F15" s="36"/>
+      <c r="F15" s="36">
+        <v>138846</v>
+      </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38">
         <v>45118</v>
       </c>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="49"/>
+      <c r="I15" s="39">
+        <v>2611</v>
+      </c>
+      <c r="J15" s="40">
+        <v>45118</v>
+      </c>
+      <c r="K15" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="49">
+        <v>8046</v>
+      </c>
       <c r="M15" s="42">
-        <v>0</v>
+        <f>49275+1594+6106</f>
+        <v>56975</v>
       </c>
       <c r="N15" s="43">
-        <v>0</v>
+        <v>57558</v>
       </c>
       <c r="P15" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>138846</v>
       </c>
       <c r="Q15" s="45">
         <f t="shared" si="1"/>
@@ -21413,19 +21431,19 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
-        <v>645824.5</v>
-      </c>
-      <c r="N49" s="547">
+        <v>702799.5</v>
+      </c>
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
-        <v>588502</v>
+        <v>646060</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>1517563</v>
-      </c>
-      <c r="Q49" s="559">
+        <v>1656409</v>
+      </c>
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>28972</v>
       </c>
@@ -21446,10 +21464,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>3094</v>
@@ -21504,11 +21522,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
-        <v>1234326.5</v>
-      </c>
-      <c r="N53" s="562"/>
+        <v>1348859.5</v>
+      </c>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -21747,7 +21765,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>183820.5</v>
+        <v>197476.5</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -21755,7 +21773,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>1484094</v>
+        <v>1622940</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -21763,7 +21781,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>21447</v>
+        <v>24058</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -21771,7 +21789,7 @@
       </c>
       <c r="L67" s="527">
         <f>SUM(L5:L65)-L26</f>
-        <v>105683.5</v>
+        <v>113729.5</v>
       </c>
       <c r="M67" s="150"/>
       <c r="N67" s="150"/>
@@ -21789,50 +21807,50 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="555" t="s">
+      <c r="H69" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="556"/>
+      <c r="I69" s="568"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="557">
+      <c r="K69" s="569">
         <f>I67+L67</f>
-        <v>127130.5</v>
-      </c>
-      <c r="L69" s="558"/>
+        <v>137787.5</v>
+      </c>
+      <c r="L69" s="570"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="549" t="s">
+      <c r="D70" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="549"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>1173143</v>
+        <v>1287676</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="550" t="s">
+      <c r="D71" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="550"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="101">
         <v>0</v>
       </c>
-      <c r="I71" s="551" t="s">
+      <c r="I71" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="552"/>
-      <c r="K71" s="553">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
-        <v>3993694.31</v>
-      </c>
-      <c r="L71" s="553"/>
+        <v>4108227.31</v>
+      </c>
+      <c r="L71" s="565"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -21870,19 +21888,19 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>1173143</v>
+        <v>1287676</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="554">
+      <c r="K73" s="566">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="553"/>
-      <c r="O73" s="594">
+      <c r="L73" s="565"/>
+      <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
       </c>
@@ -21902,22 +21920,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="542" t="s">
+      <c r="D75" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="543"/>
+      <c r="E75" s="555"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="544" t="s">
+      <c r="I75" s="556" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="545"/>
-      <c r="K75" s="546">
+      <c r="J75" s="557"/>
+      <c r="K75" s="558">
         <f>K71+K73</f>
-        <v>862307.27</v>
-      </c>
-      <c r="L75" s="546"/>
+        <v>976840.27</v>
+      </c>
+      <c r="L75" s="558"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -22062,6 +22080,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -22078,12 +22102,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23252,10 +23270,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="575" t="s">
+      <c r="I37" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="576"/>
+      <c r="J37" s="577"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -23274,8 +23292,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="577"/>
-      <c r="J38" s="578"/>
+      <c r="I38" s="578"/>
+      <c r="J38" s="579"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -23294,8 +23312,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="579"/>
-      <c r="J39" s="580"/>
+      <c r="I39" s="580"/>
+      <c r="J39" s="581"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -23853,10 +23871,10 @@
         <f>SUM(G3:G66)</f>
         <v>1585182.9300000004</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>121417.2</v>
@@ -23878,11 +23896,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -23893,7 +23911,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -25924,10 +25942,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="572"/>
-      <c r="J36" s="573"/>
-      <c r="K36" s="573"/>
-      <c r="L36" s="574"/>
+      <c r="I36" s="573"/>
+      <c r="J36" s="574"/>
+      <c r="K36" s="574"/>
+      <c r="L36" s="575"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -25954,10 +25972,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="572"/>
-      <c r="J37" s="573"/>
-      <c r="K37" s="573"/>
-      <c r="L37" s="574"/>
+      <c r="I37" s="573"/>
+      <c r="J37" s="574"/>
+      <c r="K37" s="574"/>
+      <c r="L37" s="575"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -26014,10 +26032,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="575" t="s">
+      <c r="I40" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="576"/>
+      <c r="J40" s="577"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -26036,8 +26054,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="577"/>
-      <c r="J41" s="578"/>
+      <c r="I41" s="578"/>
+      <c r="J41" s="579"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -26056,8 +26074,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="579"/>
-      <c r="J42" s="580"/>
+      <c r="I42" s="580"/>
+      <c r="J42" s="581"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -26561,10 +26579,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>92013.200000000012</v>
@@ -26584,11 +26602,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="583"/>
-      <c r="J68" s="584"/>
+      <c r="I68" s="584"/>
+      <c r="J68" s="585"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -26599,7 +26617,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="K69" s="1"/>
       <c r="L69" s="269"/>
       <c r="M69" s="5"/>
@@ -27230,23 +27248,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -27256,24 +27274,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="536" t="s">
+      <c r="R3" s="548" t="s">
         <v>3</v>
       </c>
     </row>
@@ -27288,14 +27306,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -27305,11 +27323,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="537"/>
+      <c r="R4" s="549"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -29285,11 +29303,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -29297,7 +29315,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -29330,10 +29348,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -29424,11 +29442,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -29987,26 +30005,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="555" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="556"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="557">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="558"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="549" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="549"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -30015,22 +30033,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="550" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="550"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="551" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="552"/>
-      <c r="K79" s="553">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="553"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -30071,11 +30089,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="554">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="553"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -30092,22 +30110,22 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="542" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="543"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
-      <c r="I83" s="587" t="s">
+      <c r="I83" s="588" t="s">
         <v>25</v>
       </c>
-      <c r="J83" s="588"/>
-      <c r="K83" s="589">
+      <c r="J83" s="589"/>
+      <c r="K83" s="590">
         <f>K79+K81</f>
         <v>442343.48</v>
       </c>
-      <c r="L83" s="589"/>
+      <c r="L83" s="590"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -30254,6 +30272,12 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -30270,12 +30294,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -31687,10 +31705,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="572"/>
-      <c r="J36" s="573"/>
-      <c r="K36" s="573"/>
-      <c r="L36" s="574"/>
+      <c r="I36" s="573"/>
+      <c r="J36" s="574"/>
+      <c r="K36" s="574"/>
+      <c r="L36" s="575"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -31717,10 +31735,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="572"/>
-      <c r="J37" s="573"/>
-      <c r="K37" s="573"/>
-      <c r="L37" s="574"/>
+      <c r="I37" s="573"/>
+      <c r="J37" s="574"/>
+      <c r="K37" s="574"/>
+      <c r="L37" s="575"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -31787,10 +31805,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="575" t="s">
+      <c r="I40" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="576"/>
+      <c r="J40" s="577"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -31809,8 +31827,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="577"/>
-      <c r="J41" s="578"/>
+      <c r="I41" s="578"/>
+      <c r="J41" s="579"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -31829,8 +31847,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="579"/>
-      <c r="J42" s="580"/>
+      <c r="I42" s="580"/>
+      <c r="J42" s="581"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -32334,10 +32352,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>111122</v>
@@ -32357,11 +32375,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -32372,7 +32390,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -32987,23 +33005,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -33013,24 +33031,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="592" t="s">
+      <c r="R3" s="593" t="s">
         <v>3</v>
       </c>
     </row>
@@ -33045,14 +33063,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -33062,11 +33080,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="593"/>
+      <c r="R4" s="594"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -35047,11 +35065,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -35059,7 +35077,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -35092,10 +35110,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -35186,11 +35204,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -35669,26 +35687,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="555" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="556"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="557">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="558"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="549" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="549"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -35697,22 +35715,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="550" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="550"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="551" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="552"/>
-      <c r="K79" s="553">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="553"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -35753,11 +35771,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="554">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="553"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -35774,22 +35792,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="542" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="543"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="544" t="s">
+      <c r="I83" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="545"/>
-      <c r="K83" s="546">
+      <c r="J83" s="557"/>
+      <c r="K83" s="558">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="546"/>
+      <c r="L83" s="558"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -35936,12 +35954,6 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -35958,6 +35970,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -37260,10 +37278,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="572"/>
-      <c r="J36" s="573"/>
-      <c r="K36" s="573"/>
-      <c r="L36" s="574"/>
+      <c r="I36" s="573"/>
+      <c r="J36" s="574"/>
+      <c r="K36" s="574"/>
+      <c r="L36" s="575"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -37280,10 +37298,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="572"/>
-      <c r="J37" s="573"/>
-      <c r="K37" s="573"/>
-      <c r="L37" s="574"/>
+      <c r="I37" s="573"/>
+      <c r="J37" s="574"/>
+      <c r="K37" s="574"/>
+      <c r="L37" s="575"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -37340,10 +37358,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="575" t="s">
+      <c r="I40" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="576"/>
+      <c r="J40" s="577"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -37362,8 +37380,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="577"/>
-      <c r="J41" s="578"/>
+      <c r="I41" s="578"/>
+      <c r="J41" s="579"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -37382,8 +37400,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="579"/>
-      <c r="J42" s="580"/>
+      <c r="I42" s="580"/>
+      <c r="J42" s="581"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -37887,10 +37905,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>103441.83</v>
@@ -37910,11 +37928,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -37925,7 +37943,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -38531,23 +38549,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -38557,24 +38575,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="592" t="s">
+      <c r="R3" s="593" t="s">
         <v>3</v>
       </c>
     </row>
@@ -38589,14 +38607,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -38606,11 +38624,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="593"/>
+      <c r="R4" s="594"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -40631,11 +40649,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -40643,7 +40661,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -40670,10 +40688,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -40747,11 +40765,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -41380,26 +41398,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="555" t="s">
+      <c r="H79" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="556"/>
+      <c r="I79" s="568"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="557">
+      <c r="K79" s="569">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="558"/>
+      <c r="L79" s="570"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="549" t="s">
+      <c r="D80" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="549"/>
+      <c r="E80" s="561"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -41408,22 +41426,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="550" t="s">
+      <c r="D81" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="550"/>
+      <c r="E81" s="562"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="551" t="s">
+      <c r="I81" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="552"/>
-      <c r="K81" s="553">
+      <c r="J81" s="564"/>
+      <c r="K81" s="565">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="553"/>
+      <c r="L81" s="565"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -41464,11 +41482,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="554">
+      <c r="K83" s="566">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="553"/>
+      <c r="L83" s="565"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -41485,22 +41503,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="542" t="s">
+      <c r="D85" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="543"/>
+      <c r="E85" s="555"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="544" t="s">
+      <c r="I85" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="545"/>
-      <c r="K85" s="546">
+      <c r="J85" s="557"/>
+      <c r="K85" s="558">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="546"/>
+      <c r="L85" s="558"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -41648,6 +41666,12 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -41664,12 +41688,6 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42989,10 +43007,10 @@
         <f t="shared" si="0"/>
         <v>10327.200000000001</v>
       </c>
-      <c r="I36" s="572"/>
-      <c r="J36" s="573"/>
-      <c r="K36" s="573"/>
-      <c r="L36" s="574"/>
+      <c r="I36" s="573"/>
+      <c r="J36" s="574"/>
+      <c r="K36" s="574"/>
+      <c r="L36" s="575"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -43015,10 +43033,10 @@
         <f t="shared" si="0"/>
         <v>63383.41</v>
       </c>
-      <c r="I37" s="572"/>
-      <c r="J37" s="573"/>
-      <c r="K37" s="573"/>
-      <c r="L37" s="574"/>
+      <c r="I37" s="573"/>
+      <c r="J37" s="574"/>
+      <c r="K37" s="574"/>
+      <c r="L37" s="575"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -43093,10 +43111,10 @@
         <f t="shared" si="0"/>
         <v>10162.64</v>
       </c>
-      <c r="I40" s="575" t="s">
+      <c r="I40" s="576" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="576"/>
+      <c r="J40" s="577"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -43121,8 +43139,8 @@
         <f t="shared" si="0"/>
         <v>12934.8</v>
       </c>
-      <c r="I41" s="577"/>
-      <c r="J41" s="578"/>
+      <c r="I41" s="578"/>
+      <c r="J41" s="579"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -43147,8 +43165,8 @@
         <f t="shared" si="0"/>
         <v>35275.5</v>
       </c>
-      <c r="I42" s="579"/>
-      <c r="J42" s="580"/>
+      <c r="I42" s="580"/>
+      <c r="J42" s="581"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -43670,10 +43688,10 @@
         <f>SUM(G3:G66)</f>
         <v>1592169.2799999998</v>
       </c>
-      <c r="I67" s="581" t="s">
+      <c r="I67" s="582" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="582"/>
+      <c r="J67" s="583"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>121598</v>
@@ -43693,11 +43711,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="585" t="s">
+      <c r="G68" s="586" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="590"/>
-      <c r="J68" s="591"/>
+      <c r="I68" s="591"/>
+      <c r="J68" s="592"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -43708,7 +43726,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="586"/>
+      <c r="G69" s="587"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -44324,23 +44342,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="565"/>
-      <c r="C1" s="567" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="568"/>
-      <c r="E1" s="568"/>
-      <c r="F1" s="568"/>
-      <c r="G1" s="568"/>
-      <c r="H1" s="568"/>
-      <c r="I1" s="568"/>
-      <c r="J1" s="568"/>
-      <c r="K1" s="568"/>
-      <c r="L1" s="568"/>
-      <c r="M1" s="568"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="566"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -44350,27 +44368,27 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="569" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="570"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="571" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="571"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="563" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
         <v>509</v>
       </c>
-      <c r="R3" s="592" t="s">
+      <c r="R3" s="593" t="s">
         <v>3</v>
       </c>
     </row>
@@ -44385,14 +44403,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="538" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="539"/>
-      <c r="H4" s="540" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="541"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -44402,11 +44420,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="564"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="593"/>
+      <c r="R4" s="594"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -46409,11 +46427,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="547">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="547">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -46421,7 +46439,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="559">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -46454,10 +46472,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="548"/>
-      <c r="N50" s="548"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="560"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -46536,11 +46554,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="561">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="562"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -47019,26 +47037,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="555" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="556"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="557">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="558"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="549" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="549"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -47047,22 +47065,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="550" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="550"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="551" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="552"/>
-      <c r="K79" s="553">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="553"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -47103,11 +47121,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="554">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="553"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -47124,22 +47142,22 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="542" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="543"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
-      <c r="I83" s="587" t="s">
+      <c r="I83" s="588" t="s">
         <v>25</v>
       </c>
-      <c r="J83" s="588"/>
-      <c r="K83" s="589">
+      <c r="J83" s="589"/>
+      <c r="K83" s="590">
         <f>K79+K81</f>
         <v>1169749.54</v>
       </c>
-      <c r="L83" s="589"/>
+      <c r="L83" s="590"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -47287,12 +47305,6 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47309,6 +47321,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 30 AGO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21135" windowHeight="11715" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21135" windowHeight="11715" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="  E N E R O    2 0 2 3     " sheetId="2" r:id="rId1"/>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="790">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2895,6 +2895,21 @@
   </si>
   <si>
     <t xml:space="preserve">DOCUMENTO ZAVALETA </t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-SAL</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS-JAMON-SALSAS</t>
+  </si>
+  <si>
+    <t>MAIZ-JAMON-POLLO-QUESOS-MOLE-SALCHICHA</t>
+  </si>
+  <si>
+    <t>NOMINA # 28</t>
+  </si>
+  <si>
+    <t>PASTOR--ARABE-QUESOS-JAMON-CHISTORRA-CHORIZO</t>
   </si>
 </sst>
 </file>
@@ -5588,39 +5603,6 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5695,6 +5677,39 @@
     </xf>
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9147,23 +9162,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -9173,24 +9188,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="548" t="s">
+      <c r="R3" s="537" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9205,14 +9220,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -9222,11 +9237,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="549"/>
+      <c r="R4" s="538"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -11061,11 +11076,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -11073,7 +11088,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -11094,10 +11109,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -11152,11 +11167,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -11581,26 +11596,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="567" t="s">
+      <c r="H77" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="568"/>
+      <c r="I77" s="557"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="569">
+      <c r="K77" s="558">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="570"/>
+      <c r="L77" s="559"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="561" t="s">
+      <c r="D78" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="561"/>
+      <c r="E78" s="550"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -11609,22 +11624,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="562" t="s">
+      <c r="D79" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="562"/>
+      <c r="E79" s="551"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="563" t="s">
+      <c r="I79" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="564"/>
-      <c r="K79" s="565">
+      <c r="J79" s="553"/>
+      <c r="K79" s="554">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="565"/>
+      <c r="L79" s="554"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -11665,11 +11680,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="566">
+      <c r="K81" s="555">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="565"/>
+      <c r="L81" s="554"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -11686,22 +11701,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="554" t="s">
+      <c r="D83" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="555"/>
+      <c r="E83" s="544"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="556" t="s">
+      <c r="I83" s="545" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="557"/>
-      <c r="K83" s="558">
+      <c r="J83" s="546"/>
+      <c r="K83" s="547">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="558"/>
+      <c r="L83" s="547"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -11848,6 +11863,12 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -11864,12 +11885,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14268,23 +14283,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -14294,21 +14309,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -14329,14 +14344,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -14346,7 +14361,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -16406,11 +16421,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -16418,7 +16433,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -16451,10 +16466,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -16539,11 +16554,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -16872,26 +16887,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="567" t="s">
+      <c r="H69" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="568"/>
+      <c r="I69" s="557"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="569">
+      <c r="K69" s="558">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="570"/>
+      <c r="L69" s="559"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="561" t="s">
+      <c r="D70" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="561"/>
+      <c r="E70" s="550"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -16900,23 +16915,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="562" t="s">
+      <c r="D71" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="562"/>
+      <c r="E71" s="551"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="563" t="s">
+      <c r="I71" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="564"/>
-      <c r="K71" s="565">
+      <c r="J71" s="553"/>
+      <c r="K71" s="554">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="565"/>
+      <c r="L71" s="554"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -16958,11 +16973,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="566">
+      <c r="K73" s="555">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="565"/>
+      <c r="L73" s="554"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -16979,22 +16994,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="544"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="545" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="546"/>
+      <c r="K75" s="547">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="547"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -17142,12 +17157,6 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -17164,6 +17173,12 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19536,8 +19551,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19563,23 +19578,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -19589,21 +19604,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -19622,14 +19637,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -19639,7 +19654,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -20227,7 +20242,7 @@
       <c r="U15" s="233"/>
       <c r="V15" s="233"/>
     </row>
-    <row r="16" spans="1:22" ht="26.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="504" t="s">
         <v>653</v>
       </c>
@@ -20293,37 +20308,46 @@
       <c r="B17" s="32">
         <v>45120</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="47"/>
+      <c r="C17" s="33">
+        <v>3833</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>785</v>
+      </c>
       <c r="E17" s="35">
         <v>45120</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="36">
+        <v>123280</v>
+      </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38">
         <v>45120</v>
       </c>
-      <c r="I17" s="39"/>
+      <c r="I17" s="39">
+        <v>1075</v>
+      </c>
       <c r="J17" s="40"/>
       <c r="K17" s="65"/>
       <c r="L17" s="55"/>
       <c r="M17" s="42">
-        <v>0</v>
+        <f>6664.66+66024</f>
+        <v>72688.66</v>
       </c>
       <c r="N17" s="43">
-        <v>0</v>
+        <v>45684</v>
       </c>
       <c r="O17" s="499"/>
       <c r="P17" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>123280.66</v>
       </c>
       <c r="Q17" s="45">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="46">
-        <v>0</v>
+        <v>0.66000000000349246</v>
+      </c>
+      <c r="R17" s="46" t="s">
+        <v>10</v>
       </c>
       <c r="S17" s="233"/>
       <c r="T17" s="233"/>
@@ -20337,29 +20361,38 @@
       <c r="B18" s="32">
         <v>45121</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="33">
+        <v>14381</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>786</v>
+      </c>
       <c r="E18" s="35">
         <v>45121</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="36">
+        <v>161578</v>
+      </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38">
         <v>45121</v>
       </c>
-      <c r="I18" s="39"/>
+      <c r="I18" s="39">
+        <v>1927</v>
+      </c>
       <c r="J18" s="40"/>
       <c r="K18" s="58"/>
       <c r="L18" s="49"/>
       <c r="M18" s="42">
-        <v>0</v>
+        <f>92824+5932</f>
+        <v>98756</v>
       </c>
       <c r="N18" s="43">
-        <v>0</v>
+        <v>46514</v>
       </c>
       <c r="P18" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>161578</v>
       </c>
       <c r="Q18" s="45">
         <f t="shared" si="1"/>
@@ -20380,30 +20413,45 @@
       <c r="B19" s="32">
         <v>45122</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="33">
+        <v>11918</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>787</v>
+      </c>
       <c r="E19" s="35">
         <v>45122</v>
       </c>
-      <c r="F19" s="36"/>
+      <c r="F19" s="36">
+        <v>169322</v>
+      </c>
       <c r="G19" s="37"/>
       <c r="H19" s="38">
         <v>45122</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="344"/>
-      <c r="L19" s="59"/>
+      <c r="I19" s="39">
+        <v>6179</v>
+      </c>
+      <c r="J19" s="40">
+        <v>45122</v>
+      </c>
+      <c r="K19" s="344" t="s">
+        <v>788</v>
+      </c>
+      <c r="L19" s="59">
+        <v>22183</v>
+      </c>
       <c r="M19" s="42">
-        <v>0</v>
+        <f>59255</f>
+        <v>59255</v>
       </c>
       <c r="N19" s="43">
-        <v>0</v>
+        <v>69787</v>
       </c>
       <c r="O19" s="499"/>
       <c r="P19" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>169322</v>
       </c>
       <c r="Q19" s="45">
         <f t="shared" si="1"/>
@@ -20424,29 +20472,38 @@
       <c r="B20" s="32">
         <v>45123</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="47"/>
+      <c r="C20" s="33">
+        <f>14885+6185</f>
+        <v>21070</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>789</v>
+      </c>
       <c r="E20" s="35">
         <v>45123</v>
       </c>
-      <c r="F20" s="36"/>
+      <c r="F20" s="36">
+        <v>134627</v>
+      </c>
       <c r="G20" s="37"/>
       <c r="H20" s="38">
         <v>45123</v>
       </c>
-      <c r="I20" s="39"/>
+      <c r="I20" s="39">
+        <v>1320</v>
+      </c>
       <c r="J20" s="40"/>
       <c r="K20" s="60"/>
       <c r="L20" s="55"/>
       <c r="M20" s="42">
-        <v>0</v>
+        <v>53178</v>
       </c>
       <c r="N20" s="43">
-        <v>0</v>
+        <v>59059</v>
       </c>
       <c r="P20" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>134627</v>
       </c>
       <c r="Q20" s="45">
         <f t="shared" si="1"/>
@@ -21004,12 +21061,11 @@
         <v>0</v>
       </c>
       <c r="P34" s="69">
-        <f t="shared" si="0"/>
-        <v>28972</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="45">
         <f t="shared" si="1"/>
-        <v>28972</v>
+        <v>0</v>
       </c>
       <c r="R34" s="46">
         <v>0</v>
@@ -21064,9 +21120,15 @@
       <c r="G36" s="92"/>
       <c r="H36" s="38"/>
       <c r="I36" s="39"/>
-      <c r="J36" s="338"/>
-      <c r="K36" s="88"/>
-      <c r="L36" s="49"/>
+      <c r="J36" s="338">
+        <v>45122</v>
+      </c>
+      <c r="K36" s="88" t="s">
+        <v>788</v>
+      </c>
+      <c r="L36" s="49">
+        <v>30176</v>
+      </c>
       <c r="M36" s="42">
         <v>0</v>
       </c>
@@ -21451,21 +21513,21 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
-        <v>967874</v>
-      </c>
-      <c r="N49" s="559">
+        <v>1251751.6600000001</v>
+      </c>
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
-        <v>692706</v>
+        <v>913750</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>2274936</v>
-      </c>
-      <c r="Q49" s="571">
+        <v>2834771.66</v>
+      </c>
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
-        <v>28972</v>
+        <v>0.66000000000349246</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -21484,10 +21546,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>440369</v>
@@ -21542,11 +21604,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
-        <v>1660580</v>
-      </c>
-      <c r="N53" s="538"/>
+        <v>2165501.66</v>
+      </c>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -21785,7 +21847,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>209979.5</v>
+        <v>261181.5</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -21793,7 +21855,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>1804192</v>
+        <v>2392999</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -21801,7 +21863,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>25068.5</v>
+        <v>35569.5</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -21809,7 +21871,7 @@
       </c>
       <c r="L67" s="527">
         <f>SUM(L5:L65)-L26</f>
-        <v>407022.5</v>
+        <v>459381.5</v>
       </c>
       <c r="M67" s="150"/>
       <c r="N67" s="150"/>
@@ -21827,50 +21889,50 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="567" t="s">
+      <c r="H69" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="568"/>
+      <c r="I69" s="557"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="569">
+      <c r="K69" s="558">
         <f>I67+L67</f>
-        <v>432091</v>
-      </c>
-      <c r="L69" s="570"/>
+        <v>494951</v>
+      </c>
+      <c r="L69" s="559"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="561" t="s">
+      <c r="D70" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="561"/>
+      <c r="E70" s="550"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>1162121.5</v>
+        <v>1636866.5</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="562" t="s">
+      <c r="D71" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="562"/>
+      <c r="E71" s="551"/>
       <c r="F71" s="101">
         <v>0</v>
       </c>
-      <c r="I71" s="563" t="s">
+      <c r="I71" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="564"/>
-      <c r="K71" s="565">
+      <c r="J71" s="553"/>
+      <c r="K71" s="554">
         <f>F73+F74+F75</f>
-        <v>3982672.81</v>
-      </c>
-      <c r="L71" s="565"/>
+        <v>4457417.8100000005</v>
+      </c>
+      <c r="L71" s="554"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -21908,18 +21970,18 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>1162121.5</v>
+        <v>1636866.5</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="566">
+      <c r="K73" s="555">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="565"/>
+      <c r="L73" s="554"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -21940,22 +22002,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="544"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="545" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="546"/>
+      <c r="K75" s="547">
         <f>K71+K73</f>
-        <v>851285.77</v>
-      </c>
-      <c r="L75" s="558"/>
+        <v>1326030.7700000005</v>
+      </c>
+      <c r="L75" s="547"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -22100,12 +22162,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -22122,6 +22178,12 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27268,23 +27330,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -27294,24 +27356,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="548" t="s">
+      <c r="R3" s="537" t="s">
         <v>3</v>
       </c>
     </row>
@@ -27326,14 +27388,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -27343,11 +27405,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="549"/>
+      <c r="R4" s="538"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -29323,11 +29385,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -29335,7 +29397,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -29368,10 +29430,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -29462,11 +29524,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -30025,26 +30087,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="567" t="s">
+      <c r="H77" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="568"/>
+      <c r="I77" s="557"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="569">
+      <c r="K77" s="558">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="570"/>
+      <c r="L77" s="559"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="561" t="s">
+      <c r="D78" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="561"/>
+      <c r="E78" s="550"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -30053,22 +30115,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="562" t="s">
+      <c r="D79" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="562"/>
+      <c r="E79" s="551"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="563" t="s">
+      <c r="I79" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="564"/>
-      <c r="K79" s="565">
+      <c r="J79" s="553"/>
+      <c r="K79" s="554">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="565"/>
+      <c r="L79" s="554"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -30109,11 +30171,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="566">
+      <c r="K81" s="555">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="565"/>
+      <c r="L81" s="554"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -30130,10 +30192,10 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="554" t="s">
+      <c r="D83" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="555"/>
+      <c r="E83" s="544"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
@@ -30292,12 +30354,6 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -30314,6 +30370,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33025,23 +33087,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -33051,21 +33113,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="593" t="s">
@@ -33083,14 +33145,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -33100,7 +33162,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -35085,11 +35147,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -35097,7 +35159,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -35130,10 +35192,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -35224,11 +35286,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -35707,26 +35769,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="567" t="s">
+      <c r="H77" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="568"/>
+      <c r="I77" s="557"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="569">
+      <c r="K77" s="558">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="570"/>
+      <c r="L77" s="559"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="561" t="s">
+      <c r="D78" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="561"/>
+      <c r="E78" s="550"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -35735,22 +35797,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="562" t="s">
+      <c r="D79" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="562"/>
+      <c r="E79" s="551"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="563" t="s">
+      <c r="I79" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="564"/>
-      <c r="K79" s="565">
+      <c r="J79" s="553"/>
+      <c r="K79" s="554">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="565"/>
+      <c r="L79" s="554"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -35791,11 +35853,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="566">
+      <c r="K81" s="555">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="565"/>
+      <c r="L81" s="554"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -35812,22 +35874,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="554" t="s">
+      <c r="D83" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="555"/>
+      <c r="E83" s="544"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="556" t="s">
+      <c r="I83" s="545" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="557"/>
-      <c r="K83" s="558">
+      <c r="J83" s="546"/>
+      <c r="K83" s="547">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="558"/>
+      <c r="L83" s="547"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -35974,6 +36036,12 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -35990,12 +36058,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38569,23 +38631,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -38595,21 +38657,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="593" t="s">
@@ -38627,14 +38689,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -38644,7 +38706,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -40669,11 +40731,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -40681,7 +40743,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -40708,10 +40770,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -40785,11 +40847,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -41418,26 +41480,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="567" t="s">
+      <c r="H79" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="568"/>
+      <c r="I79" s="557"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="569">
+      <c r="K79" s="558">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="570"/>
+      <c r="L79" s="559"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="561" t="s">
+      <c r="D80" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="561"/>
+      <c r="E80" s="550"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -41446,22 +41508,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="562" t="s">
+      <c r="D81" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="562"/>
+      <c r="E81" s="551"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="563" t="s">
+      <c r="I81" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="564"/>
-      <c r="K81" s="565">
+      <c r="J81" s="553"/>
+      <c r="K81" s="554">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="565"/>
+      <c r="L81" s="554"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -41502,11 +41564,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="566">
+      <c r="K83" s="555">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="565"/>
+      <c r="L83" s="554"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -41523,22 +41585,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="554" t="s">
+      <c r="D85" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="555"/>
+      <c r="E85" s="544"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="556" t="s">
+      <c r="I85" s="545" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="557"/>
-      <c r="K85" s="558">
+      <c r="J85" s="546"/>
+      <c r="K85" s="547">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="558"/>
+      <c r="L85" s="547"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -41686,12 +41748,6 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -41708,6 +41764,12 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44362,23 +44424,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="541"/>
-      <c r="C1" s="543" t="s">
+      <c r="B1" s="566"/>
+      <c r="C1" s="568" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="544"/>
-      <c r="E1" s="544"/>
-      <c r="F1" s="544"/>
-      <c r="G1" s="544"/>
-      <c r="H1" s="544"/>
-      <c r="I1" s="544"/>
-      <c r="J1" s="544"/>
-      <c r="K1" s="544"/>
-      <c r="L1" s="544"/>
-      <c r="M1" s="544"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
+      <c r="L1" s="569"/>
+      <c r="M1" s="569"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="542"/>
+      <c r="B2" s="567"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -44388,21 +44450,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="545" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="546"/>
+      <c r="B3" s="570" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="547" t="s">
+      <c r="H3" s="572" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="547"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="539" t="s">
+      <c r="P3" s="564" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -44423,14 +44485,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="550" t="s">
+      <c r="E4" s="539" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="551"/>
-      <c r="H4" s="552" t="s">
+      <c r="F4" s="540"/>
+      <c r="H4" s="541" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="542"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -44440,7 +44502,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="540"/>
+      <c r="P4" s="565"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -46447,11 +46509,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="559">
+      <c r="M49" s="548">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="559">
+      <c r="N49" s="548">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -46459,7 +46521,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="571">
+      <c r="Q49" s="560">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -46492,10 +46554,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="560"/>
-      <c r="N50" s="560"/>
+      <c r="M50" s="549"/>
+      <c r="N50" s="549"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="572"/>
+      <c r="Q50" s="561"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -46574,11 +46636,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="537">
+      <c r="M53" s="562">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="538"/>
+      <c r="N53" s="563"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -47057,26 +47119,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="567" t="s">
+      <c r="H77" s="556" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="568"/>
+      <c r="I77" s="557"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="569">
+      <c r="K77" s="558">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="570"/>
+      <c r="L77" s="559"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="561" t="s">
+      <c r="D78" s="550" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="561"/>
+      <c r="E78" s="550"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -47085,22 +47147,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="562" t="s">
+      <c r="D79" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="562"/>
+      <c r="E79" s="551"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="563" t="s">
+      <c r="I79" s="552" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="564"/>
-      <c r="K79" s="565">
+      <c r="J79" s="553"/>
+      <c r="K79" s="554">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="565"/>
+      <c r="L79" s="554"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -47141,11 +47203,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="566">
+      <c r="K81" s="555">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="565"/>
+      <c r="L81" s="554"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -47162,10 +47224,10 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="554" t="s">
+      <c r="D83" s="543" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="555"/>
+      <c r="E83" s="544"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
@@ -47325,6 +47387,12 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47341,12 +47409,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 31 AGO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  ZAVALETA   JULIO    2023.xlsx
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="805">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2910,6 +2910,51 @@
   </si>
   <si>
     <t>PASTOR--ARABE-QUESOS-JAMON-CHISTORRA-CHORIZO</t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-CHORIZO-JAMON-SALCHICHA</t>
+  </si>
+  <si>
+    <t>BIMBO-QUESOS-POLLO-JAMON-LONGANIZA</t>
+  </si>
+  <si>
+    <t>ALBICIA Nota 3492</t>
+  </si>
+  <si>
+    <t>ALBICIA Nota 4153</t>
+  </si>
+  <si>
+    <t>ALBICIA Nota 4812</t>
+  </si>
+  <si>
+    <t>ALBICIA Nota 4952</t>
+  </si>
+  <si>
+    <t>Licencia Zavaleta</t>
+  </si>
+  <si>
+    <t>BIMBO-PASTOR-POLLO-QUESOS-CEBOLLA</t>
+  </si>
+  <si>
+    <t>QUESOS-JAMON-POLLO-SALCHICAS-NATA</t>
+  </si>
+  <si>
+    <t>NOMINA # 29</t>
+  </si>
+  <si>
+    <t>PASTOR-QUESOS-CHISTORRA-JAMON</t>
+  </si>
+  <si>
+    <t>CHORIZO-SALCHICHA-MAIZ-JAMON-QUESOS-POLLO</t>
+  </si>
+  <si>
+    <t>BIMBO-SALCHICHA-SALMON-QUESOS-POLLO-SALSAS</t>
+  </si>
+  <si>
+    <t>POLLO-ROASBEF-QUSOS-ARABE</t>
+  </si>
+  <si>
+    <t>SAL-PASTOR-POLLO</t>
   </si>
 </sst>
 </file>
@@ -4593,7 +4638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="595">
+  <cellXfs count="596">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5603,6 +5648,39 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5678,39 +5756,6 @@
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5776,6 +5821,9 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9162,23 +9210,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -9188,24 +9236,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="537" t="s">
+      <c r="R3" s="548" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9220,14 +9268,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -9237,11 +9285,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="538"/>
+      <c r="R4" s="549"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -11076,11 +11124,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -11088,7 +11136,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -11109,10 +11157,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -11167,11 +11215,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -11596,26 +11644,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="556" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="557"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="558">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="559"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="550" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="550"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -11624,22 +11672,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="551" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="551"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="552" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="553"/>
-      <c r="K79" s="554">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="554"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -11680,11 +11728,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="555">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="554"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -11701,22 +11749,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="543" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="544"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="545" t="s">
+      <c r="I83" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="546"/>
-      <c r="K83" s="547">
+      <c r="J83" s="557"/>
+      <c r="K83" s="558">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="547"/>
+      <c r="L83" s="558"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -11863,12 +11911,6 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -11885,6 +11927,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14283,23 +14331,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -14309,21 +14357,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -14344,14 +14392,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -14361,7 +14409,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -16421,11 +16469,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -16433,7 +16481,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -16466,10 +16514,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -16554,11 +16602,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -16887,26 +16935,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="556" t="s">
+      <c r="H69" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="557"/>
+      <c r="I69" s="568"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="558">
+      <c r="K69" s="569">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="559"/>
+      <c r="L69" s="570"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="550" t="s">
+      <c r="D70" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="550"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -16915,23 +16963,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="551" t="s">
+      <c r="D71" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="551"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="552" t="s">
+      <c r="I71" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="553"/>
-      <c r="K71" s="554">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="554"/>
+      <c r="L71" s="565"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -16973,11 +17021,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="555">
+      <c r="K73" s="566">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="554"/>
+      <c r="L73" s="565"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -16994,22 +17042,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="543" t="s">
+      <c r="D75" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="544"/>
+      <c r="E75" s="555"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="545" t="s">
+      <c r="I75" s="556" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="546"/>
-      <c r="K75" s="547">
+      <c r="J75" s="557"/>
+      <c r="K75" s="558">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="547"/>
+      <c r="L75" s="558"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -17157,6 +17205,12 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -17173,12 +17227,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19551,8 +19599,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19578,23 +19626,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -19604,21 +19652,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
@@ -19637,14 +19685,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -19654,7 +19702,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -19703,7 +19751,7 @@
         <v>84700</v>
       </c>
       <c r="P5" s="44">
-        <f t="shared" ref="P5:P34" si="0">N5+M5+L5+I5+C5</f>
+        <f t="shared" ref="P5:P33" si="0">N5+M5+L5+I5+C5</f>
         <v>187028</v>
       </c>
       <c r="Q5" s="45">
@@ -20524,33 +20572,42 @@
       <c r="B21" s="32">
         <v>45124</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="47"/>
+      <c r="C21" s="33">
+        <v>17173</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>790</v>
+      </c>
       <c r="E21" s="35">
         <v>45124</v>
       </c>
-      <c r="F21" s="36"/>
+      <c r="F21" s="36">
+        <v>161118</v>
+      </c>
       <c r="G21" s="37"/>
       <c r="H21" s="38">
         <v>45124</v>
       </c>
-      <c r="I21" s="39"/>
+      <c r="I21" s="39">
+        <v>2328</v>
+      </c>
       <c r="J21" s="40"/>
       <c r="K21" s="402"/>
       <c r="L21" s="55"/>
       <c r="M21" s="42">
-        <v>0</v>
+        <f>95440.5+1108</f>
+        <v>96548.5</v>
       </c>
       <c r="N21" s="43">
-        <v>0</v>
+        <v>45068</v>
       </c>
       <c r="P21" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>161117.5</v>
       </c>
       <c r="Q21" s="45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R21" s="46">
         <v>0</v>
@@ -20564,29 +20621,38 @@
       <c r="B22" s="32">
         <v>45125</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="47"/>
+      <c r="C22" s="33">
+        <v>26528</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>791</v>
+      </c>
       <c r="E22" s="35">
         <v>45125</v>
       </c>
-      <c r="F22" s="36"/>
+      <c r="F22" s="36">
+        <v>247019</v>
+      </c>
       <c r="G22" s="37"/>
       <c r="H22" s="38">
         <v>45125</v>
       </c>
-      <c r="I22" s="359"/>
+      <c r="I22" s="359">
+        <v>2429</v>
+      </c>
       <c r="J22" s="40"/>
       <c r="K22" s="506"/>
       <c r="L22" s="62"/>
       <c r="M22" s="42">
-        <v>0</v>
+        <f>93028+44000</f>
+        <v>137028</v>
       </c>
       <c r="N22" s="43">
-        <v>0</v>
+        <v>81034</v>
       </c>
       <c r="P22" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>247019</v>
       </c>
       <c r="Q22" s="45">
         <f t="shared" si="1"/>
@@ -20604,33 +20670,48 @@
       <c r="B23" s="32">
         <v>45126</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="47"/>
+      <c r="C23" s="33">
+        <v>6578</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>88</v>
+      </c>
       <c r="E23" s="35">
         <v>45126</v>
       </c>
-      <c r="F23" s="36"/>
+      <c r="F23" s="36">
+        <v>212178</v>
+      </c>
       <c r="G23" s="37"/>
       <c r="H23" s="38">
         <v>45126</v>
       </c>
-      <c r="I23" s="39"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="55"/>
+      <c r="I23" s="39">
+        <v>1822</v>
+      </c>
+      <c r="J23" s="64">
+        <v>45126</v>
+      </c>
+      <c r="K23" s="65" t="s">
+        <v>796</v>
+      </c>
+      <c r="L23" s="55">
+        <v>7209</v>
+      </c>
       <c r="M23" s="42">
-        <v>0</v>
+        <f>127627+1347+4280+8806.6</f>
+        <v>142060.6</v>
       </c>
       <c r="N23" s="43">
-        <v>0</v>
+        <v>54508</v>
       </c>
       <c r="P23" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>212177.6</v>
       </c>
       <c r="Q23" s="45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.39999999999417923</v>
       </c>
       <c r="R23" s="46">
         <v>0</v>
@@ -20644,29 +20725,37 @@
       <c r="B24" s="32">
         <v>45127</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="33">
+        <v>8756</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>797</v>
+      </c>
       <c r="E24" s="35">
         <v>45127</v>
       </c>
-      <c r="F24" s="36"/>
+      <c r="F24" s="36">
+        <v>187038</v>
+      </c>
       <c r="G24" s="37"/>
       <c r="H24" s="38">
         <v>45127</v>
       </c>
-      <c r="I24" s="39"/>
+      <c r="I24" s="39">
+        <v>1963</v>
+      </c>
       <c r="J24" s="66"/>
       <c r="K24" s="65"/>
       <c r="L24" s="67"/>
       <c r="M24" s="42">
-        <v>0</v>
+        <v>110733</v>
       </c>
       <c r="N24" s="43">
-        <v>0</v>
+        <v>65586</v>
       </c>
       <c r="P24" s="49">
         <f>N24+M24+L24+I24+C24</f>
-        <v>0</v>
+        <v>187038</v>
       </c>
       <c r="Q24" s="45">
         <f t="shared" si="1"/>
@@ -20684,29 +20773,38 @@
       <c r="B25" s="32">
         <v>45128</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="47"/>
+      <c r="C25" s="33">
+        <v>19396</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>798</v>
+      </c>
       <c r="E25" s="35">
         <v>45128</v>
       </c>
-      <c r="F25" s="36"/>
+      <c r="F25" s="36">
+        <v>209280</v>
+      </c>
       <c r="G25" s="37"/>
       <c r="H25" s="38">
         <v>45128</v>
       </c>
-      <c r="I25" s="39"/>
+      <c r="I25" s="39">
+        <v>2127</v>
+      </c>
       <c r="J25" s="64"/>
       <c r="K25" s="65"/>
       <c r="L25" s="68"/>
       <c r="M25" s="42">
-        <v>0</v>
+        <f>112366+1905</f>
+        <v>114271</v>
       </c>
       <c r="N25" s="43">
-        <v>0</v>
+        <v>73486</v>
       </c>
       <c r="P25" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>209280</v>
       </c>
       <c r="Q25" s="45">
         <f t="shared" si="1"/>
@@ -20724,32 +20822,48 @@
       <c r="B26" s="32">
         <v>45129</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="47"/>
+      <c r="C26" s="33">
+        <v>11325</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>86</v>
+      </c>
       <c r="E26" s="35">
         <v>45129</v>
       </c>
-      <c r="F26" s="36"/>
+      <c r="F26" s="36">
+        <v>196587</v>
+      </c>
       <c r="G26" s="37"/>
       <c r="H26" s="38">
         <v>45129</v>
       </c>
-      <c r="I26" s="39"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="71"/>
+      <c r="I26" s="39">
+        <v>2556.5</v>
+      </c>
+      <c r="J26" s="40">
+        <v>45129</v>
+      </c>
+      <c r="K26" s="595" t="s">
+        <v>799</v>
+      </c>
+      <c r="L26" s="71">
+        <f>22683+2100</f>
+        <v>24783</v>
+      </c>
       <c r="M26" s="42">
-        <v>0</v>
+        <f>85748.5</f>
+        <v>85748.5</v>
       </c>
       <c r="N26" s="43">
-        <v>0</v>
+        <v>72174</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P26" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>196587</v>
       </c>
       <c r="Q26" s="45">
         <f t="shared" si="1"/>
@@ -20769,29 +20883,37 @@
       <c r="B27" s="32">
         <v>45130</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="33">
+        <v>19047</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>800</v>
+      </c>
       <c r="E27" s="35">
         <v>45130</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="36">
+        <v>104829</v>
+      </c>
       <c r="G27" s="37"/>
       <c r="H27" s="38">
         <v>45130</v>
       </c>
-      <c r="I27" s="39"/>
+      <c r="I27" s="39">
+        <v>1268</v>
+      </c>
       <c r="J27" s="337"/>
       <c r="K27" s="345"/>
       <c r="L27" s="68"/>
       <c r="M27" s="42">
-        <v>0</v>
+        <v>46629</v>
       </c>
       <c r="N27" s="43">
-        <v>0</v>
+        <v>37885</v>
       </c>
       <c r="P27" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>104829</v>
       </c>
       <c r="Q27" s="45">
         <f t="shared" si="1"/>
@@ -20809,29 +20931,38 @@
       <c r="B28" s="32">
         <v>45131</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="51"/>
+      <c r="C28" s="33">
+        <v>24947.5</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>801</v>
+      </c>
       <c r="E28" s="35">
         <v>45131</v>
       </c>
-      <c r="F28" s="36"/>
+      <c r="F28" s="36">
+        <v>149695</v>
+      </c>
       <c r="G28" s="37"/>
       <c r="H28" s="38">
         <v>45131</v>
       </c>
-      <c r="I28" s="39"/>
+      <c r="I28" s="39">
+        <v>2693</v>
+      </c>
       <c r="J28" s="338"/>
       <c r="K28" s="70"/>
       <c r="L28" s="68"/>
       <c r="M28" s="42">
-        <v>0</v>
+        <f>58763.5+1992</f>
+        <v>60755.5</v>
       </c>
       <c r="N28" s="43">
-        <v>0</v>
+        <v>61299</v>
       </c>
       <c r="P28" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149695</v>
       </c>
       <c r="Q28" s="45">
         <f t="shared" si="1"/>
@@ -20849,29 +20980,38 @@
       <c r="B29" s="32">
         <v>45132</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="76"/>
+      <c r="C29" s="33">
+        <v>17903</v>
+      </c>
+      <c r="D29" s="76" t="s">
+        <v>802</v>
+      </c>
       <c r="E29" s="35">
         <v>45132</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="36">
+        <v>156042</v>
+      </c>
       <c r="G29" s="37"/>
       <c r="H29" s="38">
         <v>45132</v>
       </c>
-      <c r="I29" s="39"/>
+      <c r="I29" s="39">
+        <v>1685</v>
+      </c>
       <c r="J29" s="339"/>
       <c r="K29" s="346"/>
       <c r="L29" s="68"/>
       <c r="M29" s="42">
-        <v>0</v>
+        <f>87594+321</f>
+        <v>87915</v>
       </c>
       <c r="N29" s="43">
-        <v>0</v>
+        <v>48539</v>
       </c>
       <c r="P29" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>156042</v>
       </c>
       <c r="Q29" s="45">
         <f t="shared" si="1"/>
@@ -20889,29 +21029,38 @@
       <c r="B30" s="32">
         <v>45133</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="76"/>
+      <c r="C30" s="33">
+        <v>12784</v>
+      </c>
+      <c r="D30" s="76" t="s">
+        <v>803</v>
+      </c>
       <c r="E30" s="35">
         <v>45133</v>
       </c>
-      <c r="F30" s="36"/>
+      <c r="F30" s="36">
+        <v>197865</v>
+      </c>
       <c r="G30" s="37"/>
       <c r="H30" s="38">
         <v>45133</v>
       </c>
-      <c r="I30" s="39"/>
+      <c r="I30" s="39">
+        <v>994</v>
+      </c>
       <c r="J30" s="338"/>
       <c r="K30" s="65"/>
       <c r="L30" s="49"/>
       <c r="M30" s="42">
-        <v>0</v>
+        <f>121720+6600</f>
+        <v>128320</v>
       </c>
       <c r="N30" s="43">
-        <v>0</v>
+        <v>55767</v>
       </c>
       <c r="P30" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>197865</v>
       </c>
       <c r="Q30" s="45">
         <f t="shared" si="1"/>
@@ -20929,29 +21078,37 @@
       <c r="B31" s="32">
         <v>45134</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="79"/>
+      <c r="C31" s="33">
+        <v>4749</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>804</v>
+      </c>
       <c r="E31" s="35">
         <v>45134</v>
       </c>
-      <c r="F31" s="36"/>
+      <c r="F31" s="36">
+        <v>135472</v>
+      </c>
       <c r="G31" s="37"/>
       <c r="H31" s="38">
         <v>45134</v>
       </c>
-      <c r="I31" s="39"/>
+      <c r="I31" s="39">
+        <v>2852</v>
+      </c>
       <c r="J31" s="338"/>
       <c r="K31" s="347"/>
       <c r="L31" s="68"/>
       <c r="M31" s="42">
-        <v>0</v>
+        <v>78371</v>
       </c>
       <c r="N31" s="43">
-        <v>0</v>
+        <v>49500</v>
       </c>
       <c r="P31" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>135472</v>
       </c>
       <c r="Q31" s="45">
         <f t="shared" si="1"/>
@@ -21076,9 +21233,15 @@
     </row>
     <row r="35" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="504"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="79"/>
+      <c r="B35" s="32">
+        <v>45108</v>
+      </c>
+      <c r="C35" s="86">
+        <v>9070</v>
+      </c>
+      <c r="D35" s="79" t="s">
+        <v>792</v>
+      </c>
       <c r="E35" s="35"/>
       <c r="F35" s="36"/>
       <c r="G35" s="37"/>
@@ -21112,9 +21275,15 @@
     </row>
     <row r="36" spans="1:19" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="94"/>
+      <c r="B36" s="32">
+        <v>45108</v>
+      </c>
+      <c r="C36" s="90">
+        <v>10034</v>
+      </c>
+      <c r="D36" s="94" t="s">
+        <v>793</v>
+      </c>
       <c r="E36" s="35"/>
       <c r="F36" s="36"/>
       <c r="G36" s="92"/>
@@ -21148,17 +21317,29 @@
     </row>
     <row r="37" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="94"/>
+      <c r="B37" s="32">
+        <v>45108</v>
+      </c>
+      <c r="C37" s="93">
+        <v>12993</v>
+      </c>
+      <c r="D37" s="94" t="s">
+        <v>794</v>
+      </c>
       <c r="E37" s="35"/>
       <c r="F37" s="36"/>
       <c r="G37" s="92"/>
       <c r="H37" s="38"/>
       <c r="I37" s="39"/>
-      <c r="J37" s="338"/>
-      <c r="K37" s="350"/>
-      <c r="L37" s="49"/>
+      <c r="J37" s="338">
+        <v>45129</v>
+      </c>
+      <c r="K37" s="350" t="s">
+        <v>799</v>
+      </c>
+      <c r="L37" s="49">
+        <v>29754</v>
+      </c>
       <c r="M37" s="42">
         <v>0</v>
       </c>
@@ -21178,9 +21359,15 @@
     </row>
     <row r="38" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="512"/>
+      <c r="B38" s="32">
+        <v>45108</v>
+      </c>
+      <c r="C38" s="93">
+        <v>3546</v>
+      </c>
+      <c r="D38" s="94" t="s">
+        <v>795</v>
+      </c>
       <c r="E38" s="35"/>
       <c r="F38" s="36"/>
       <c r="G38" s="92"/>
@@ -21513,21 +21700,21 @@
       <c r="J49" s="338"/>
       <c r="K49" s="343"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
-        <v>1251751.6600000001</v>
-      </c>
-      <c r="N49" s="548">
+        <v>2340131.7600000002</v>
+      </c>
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
-        <v>913750</v>
+        <v>1558596</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>2834771.66</v>
-      </c>
-      <c r="Q49" s="560">
+        <v>4791893.76</v>
+      </c>
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
-        <v>0.66000000000349246</v>
+        <v>-0.23999999999068677</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -21546,10 +21733,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>440369</v>
@@ -21604,11 +21791,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
-        <v>2165501.66</v>
-      </c>
-      <c r="N53" s="563"/>
+        <v>3898727.7600000002</v>
+      </c>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -21847,7 +22034,7 @@
       </c>
       <c r="C67" s="519">
         <f>SUM(C5:C61)</f>
-        <v>261181.5</v>
+        <v>466011</v>
       </c>
       <c r="D67" s="520"/>
       <c r="E67" s="521" t="s">
@@ -21855,7 +22042,7 @@
       </c>
       <c r="F67" s="522">
         <f>SUM(F5:F61)</f>
-        <v>2392999</v>
+        <v>4350122</v>
       </c>
       <c r="G67" s="523"/>
       <c r="H67" s="521" t="s">
@@ -21863,7 +22050,7 @@
       </c>
       <c r="I67" s="524">
         <f>SUM(I5:I61)</f>
-        <v>35569.5</v>
+        <v>58287</v>
       </c>
       <c r="J67" s="525"/>
       <c r="K67" s="526" t="s">
@@ -21871,7 +22058,7 @@
       </c>
       <c r="L67" s="527">
         <f>SUM(L5:L65)-L26</f>
-        <v>459381.5</v>
+        <v>496344.5</v>
       </c>
       <c r="M67" s="150"/>
       <c r="N67" s="150"/>
@@ -21889,50 +22076,50 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="556" t="s">
+      <c r="H69" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="557"/>
+      <c r="I69" s="568"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="558">
+      <c r="K69" s="569">
         <f>I67+L67</f>
-        <v>494951</v>
-      </c>
-      <c r="L69" s="559"/>
+        <v>554631.5</v>
+      </c>
+      <c r="L69" s="570"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="550" t="s">
+      <c r="D70" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="550"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
-        <v>1636866.5</v>
+        <v>3329479.5</v>
       </c>
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="551" t="s">
+      <c r="D71" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="551"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="101">
         <v>0</v>
       </c>
-      <c r="I71" s="552" t="s">
+      <c r="I71" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="553"/>
-      <c r="K71" s="554">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
-        <v>4457417.8100000005</v>
-      </c>
-      <c r="L71" s="554"/>
+        <v>6150030.8100000005</v>
+      </c>
+      <c r="L71" s="565"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -21970,18 +22157,18 @@
       </c>
       <c r="F73" s="150">
         <f>SUM(F70:F72)</f>
-        <v>1636866.5</v>
+        <v>3329479.5</v>
       </c>
       <c r="H73" s="168"/>
       <c r="I73" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="555">
+      <c r="K73" s="566">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="554"/>
+      <c r="L73" s="565"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -22002,22 +22189,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="543" t="s">
+      <c r="D75" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="544"/>
+      <c r="E75" s="555"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="545" t="s">
+      <c r="I75" s="556" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="546"/>
-      <c r="K75" s="547">
+      <c r="J75" s="557"/>
+      <c r="K75" s="558">
         <f>K71+K73</f>
-        <v>1326030.7700000005</v>
-      </c>
-      <c r="L75" s="547"/>
+        <v>3018643.7700000005</v>
+      </c>
+      <c r="L75" s="558"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -22162,6 +22349,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -22178,12 +22371,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27330,23 +27517,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -27356,24 +27543,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="537" t="s">
+      <c r="R3" s="548" t="s">
         <v>3</v>
       </c>
     </row>
@@ -27388,14 +27575,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -27405,11 +27592,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="538"/>
+      <c r="R4" s="549"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -29385,11 +29572,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -29397,7 +29584,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -29430,10 +29617,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -29524,11 +29711,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -30087,26 +30274,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="556" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="557"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="558">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="559"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="550" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="550"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -30115,22 +30302,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="551" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="551"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="552" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="553"/>
-      <c r="K79" s="554">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="554"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -30171,11 +30358,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="555">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="554"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -30192,10 +30379,10 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="543" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="544"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
@@ -30354,6 +30541,12 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -30370,12 +30563,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33087,23 +33274,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -33113,21 +33300,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="593" t="s">
@@ -33145,14 +33332,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -33162,7 +33349,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -35147,11 +35334,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -35159,7 +35346,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -35192,10 +35379,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -35286,11 +35473,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -35769,26 +35956,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="556" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="557"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="558">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="559"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="550" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="550"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -35797,22 +35984,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="551" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="551"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="552" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="553"/>
-      <c r="K79" s="554">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="554"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -35853,11 +36040,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="555">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="554"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -35874,22 +36061,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="543" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="544"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="545" t="s">
+      <c r="I83" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="546"/>
-      <c r="K83" s="547">
+      <c r="J83" s="557"/>
+      <c r="K83" s="558">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="547"/>
+      <c r="L83" s="558"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -36036,12 +36223,6 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -36058,6 +36239,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38631,23 +38818,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -38657,21 +38844,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="593" t="s">
@@ -38689,14 +38876,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -38706,7 +38893,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -40731,11 +40918,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -40743,7 +40930,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -40770,10 +40957,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -40847,11 +41034,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -41480,26 +41667,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="556" t="s">
+      <c r="H79" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="557"/>
+      <c r="I79" s="568"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="558">
+      <c r="K79" s="569">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="559"/>
+      <c r="L79" s="570"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="550" t="s">
+      <c r="D80" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="550"/>
+      <c r="E80" s="561"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -41508,22 +41695,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="551" t="s">
+      <c r="D81" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="551"/>
+      <c r="E81" s="562"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="552" t="s">
+      <c r="I81" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="553"/>
-      <c r="K81" s="554">
+      <c r="J81" s="564"/>
+      <c r="K81" s="565">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="554"/>
+      <c r="L81" s="565"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -41564,11 +41751,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="555">
+      <c r="K83" s="566">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="554"/>
+      <c r="L83" s="565"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -41585,22 +41772,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="543" t="s">
+      <c r="D85" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="544"/>
+      <c r="E85" s="555"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="545" t="s">
+      <c r="I85" s="556" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="546"/>
-      <c r="K85" s="547">
+      <c r="J85" s="557"/>
+      <c r="K85" s="558">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="547"/>
+      <c r="L85" s="558"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -41748,6 +41935,12 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -41764,12 +41957,6 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44424,23 +44611,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="566"/>
-      <c r="C1" s="568" t="s">
+      <c r="B1" s="541"/>
+      <c r="C1" s="543" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="569"/>
-      <c r="G1" s="569"/>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="569"/>
-      <c r="L1" s="569"/>
-      <c r="M1" s="569"/>
+      <c r="D1" s="544"/>
+      <c r="E1" s="544"/>
+      <c r="F1" s="544"/>
+      <c r="G1" s="544"/>
+      <c r="H1" s="544"/>
+      <c r="I1" s="544"/>
+      <c r="J1" s="544"/>
+      <c r="K1" s="544"/>
+      <c r="L1" s="544"/>
+      <c r="M1" s="544"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="567"/>
+      <c r="B2" s="542"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -44450,21 +44637,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="570" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="571"/>
+      <c r="B3" s="545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="546"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="572" t="s">
+      <c r="H3" s="547" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="572"/>
+      <c r="I3" s="547"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="539" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
@@ -44485,14 +44672,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="550" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="551"/>
+      <c r="H4" s="552" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="553"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -44502,7 +44689,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="540"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -46509,11 +46696,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="548">
+      <c r="M49" s="559">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="548">
+      <c r="N49" s="559">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -46521,7 +46708,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="560">
+      <c r="Q49" s="571">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -46554,10 +46741,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="549"/>
-      <c r="N50" s="549"/>
+      <c r="M50" s="560"/>
+      <c r="N50" s="560"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="561"/>
+      <c r="Q50" s="572"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -46636,11 +46823,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="562">
+      <c r="M53" s="537">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="563"/>
+      <c r="N53" s="538"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -47119,26 +47306,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="556" t="s">
+      <c r="H77" s="567" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="557"/>
+      <c r="I77" s="568"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="558">
+      <c r="K77" s="569">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="559"/>
+      <c r="L77" s="570"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="550" t="s">
+      <c r="D78" s="561" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="550"/>
+      <c r="E78" s="561"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -47147,22 +47334,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="551" t="s">
+      <c r="D79" s="562" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="551"/>
+      <c r="E79" s="562"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="552" t="s">
+      <c r="I79" s="563" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="553"/>
-      <c r="K79" s="554">
+      <c r="J79" s="564"/>
+      <c r="K79" s="565">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="554"/>
+      <c r="L79" s="565"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -47203,11 +47390,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="555">
+      <c r="K81" s="566">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="554"/>
+      <c r="L81" s="565"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -47224,10 +47411,10 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="543" t="s">
+      <c r="D83" s="554" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="544"/>
+      <c r="E83" s="555"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
@@ -47387,12 +47574,6 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47409,6 +47590,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>